<commit_message>
Added few functionalities, added APK, Assignment feature in progress
</commit_message>
<xml_diff>
--- a/app/src/main/assets/Achievements.xlsx
+++ b/app/src/main/assets/Achievements.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\AndroidStudioProjects\AcademicAlly\app\src\main\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C3574F-2997-409B-A818-DE941DC39135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235419D3-F73E-4AA8-AEFB-D17B8132731B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,14 +26,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="66">
   <si>
     <t>Collect 100 points</t>
   </si>
   <si>
-    <t>Have a rating of 5 in a course</t>
-  </si>
-  <si>
     <t>Accept a student request</t>
   </si>
   <si>
@@ -88,15 +85,6 @@
     <t>Have 10 courses eligible as tutor</t>
   </si>
   <si>
-    <t>Have a rating of 5 in 3 courses</t>
-  </si>
-  <si>
-    <t>Have a role to be tutor</t>
-  </si>
-  <si>
-    <t>Have a role to be student</t>
-  </si>
-  <si>
     <t>Request a tutoring session</t>
   </si>
   <si>
@@ -172,9 +160,6 @@
     <t>Session Expert</t>
   </si>
   <si>
-    <t>Beginner Tutor</t>
-  </si>
-  <si>
     <t>Session Maestro</t>
   </si>
   <si>
@@ -190,12 +175,6 @@
     <t>Master Tutor</t>
   </si>
   <si>
-    <t>Top-Rated Instructor</t>
-  </si>
-  <si>
-    <t>Highly Rated Mentor</t>
-  </si>
-  <si>
     <t>Learning Aspirant</t>
   </si>
   <si>
@@ -230,9 +209,6 @@
   </si>
   <si>
     <t>Educational Achiever</t>
-  </si>
-  <si>
-    <t>Beginner Student</t>
   </si>
   <si>
     <t>Session Participant</t>
@@ -565,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -580,15 +556,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -596,7 +572,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -604,7 +580,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -612,7 +588,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -620,7 +596,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -628,7 +604,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -636,7 +612,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -644,7 +620,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -652,7 +628,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -660,23 +636,23 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
@@ -684,7 +660,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
@@ -692,7 +668,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
@@ -700,7 +676,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
@@ -708,7 +684,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
@@ -716,7 +692,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
@@ -724,34 +700,10 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -761,10 +713,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B46E0685-0F6C-42F4-818D-5ECAC2ACEEBF}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -775,71 +727,71 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -847,7 +799,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -855,23 +807,23 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
@@ -879,7 +831,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
@@ -887,7 +839,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
@@ -895,42 +847,34 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>73</v>
-      </c>
-      <c r="B20" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>